<commit_message>
Correção no form A, Estilização Expansão MS
</commit_message>
<xml_diff>
--- a/inputs/0 - Belém/0 - Monitoramento Form 1, 2 e 3.xlsx
+++ b/inputs/0 - Belém/0 - Monitoramento Form 1, 2 e 3.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29324"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F7354D6B2CFE853A586A6581DC9AA9CC4624A815" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{318DA43B-2D3E-4227-B8D0-021B58C862F6}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_F7354D6B2C4E814D78097D81DC9AA9CC4624A815" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E3DD3A2-AACD-47A9-BF4F-629595257D06}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>